<commit_message>
hundles signal without spkikes
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Feature_5</t>
+          <t>average_of_num_of_spikes</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -477,20 +477,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>254</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
       <c r="D2" t="n">
-        <v>-5.323915901574802e-05</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>24413.85770750988</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -500,20 +502,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
       <c r="D3" t="n">
-        <v>2.372602043478261e-05</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>252678.5</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -523,18 +527,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
       <c r="D4" t="n">
-        <v>2.249865e-05</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -719,22 +727,20 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>-3.301043592334494e-05</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>21388</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -746,14 +752,12 @@
       <c r="B13" t="n">
         <v>355</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="n">
         <v>-6.969021709859154e-05</v>
       </c>
-      <c r="D13" t="n">
-        <v>4</v>
-      </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>17087.58474576271</v>
       </c>
       <c r="F13" t="n">
         <v>4</v>
@@ -771,17 +775,15 @@
       <c r="B14" t="n">
         <v>99</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="n">
         <v>2.583738818181818e-05</v>
       </c>
-      <c r="D14" t="n">
-        <v>5</v>
-      </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>60780.57142857143</v>
       </c>
       <c r="F14" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -796,17 +798,15 @@
       <c r="B15" t="n">
         <v>651</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="n">
         <v>3.238886926267281e-05</v>
       </c>
-      <c r="D15" t="n">
-        <v>5</v>
-      </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>9513.453846153847</v>
       </c>
       <c r="F15" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -822,16 +822,16 @@
         <v>143</v>
       </c>
       <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
         <v>-2.794813909090908e-05</v>
       </c>
-      <c r="D16" t="n">
-        <v>5</v>
-      </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>42993.64084507043</v>
       </c>
       <c r="F16" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -856,10 +856,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -869,22 +869,20 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>-2.594931e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>2716515.5</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -959,6 +957,2506 @@
         <v>0</v>
       </c>
       <c r="G21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Electrode_21</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Electrode_22</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Electrode_23</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Electrode_24</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Electrode_25</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Electrode_26</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Electrode_27</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Electrode_28</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Electrode_29</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Electrode_30</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Electrode_31</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Electrode_32</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Electrode_33</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Electrode_34</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Electrode_35</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Electrode_36</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Electrode_37</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Electrode_38</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Electrode_39</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Electrode_40</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Electrode_41</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Electrode_42</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Electrode_43</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Electrode_44</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Electrode_45</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Electrode_46</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Electrode_47</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Electrode_48</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Electrode_49</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Electrode_50</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Electrode_51</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Electrode_52</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Electrode_53</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Electrode_54</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Electrode_55</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Electrode_56</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Electrode_57</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Electrode_58</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Electrode_59</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Electrode_60</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Electrode_61</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Electrode_62</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Electrode_63</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Electrode_64</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Electrode_65</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Electrode_66</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Electrode_67</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Electrode_68</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Electrode_69</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Electrode_70</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Electrode_71</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Electrode_72</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Electrode_73</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Electrode_74</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Electrode_75</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Electrode_76</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Electrode_77</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Electrode_78</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Electrode_79</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Electrode_80</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Electrode_81</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Electrode_82</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Electrode_83</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Electrode_84</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Electrode_85</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Electrode_86</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Electrode_87</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Electrode_88</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Electrode_89</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Electrode_90</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Electrode_91</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Electrode_92</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>0</v>
+      </c>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Electrode_93</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Electrode_94</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Electrode_95</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Electrode_96</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0</v>
+      </c>
+      <c r="C97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Electrode_97</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Electrode_98</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Electrode_99</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Electrode_100</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Electrode_101</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0</v>
+      </c>
+      <c r="G102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Electrode_102</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Electrode_103</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0</v>
+      </c>
+      <c r="G104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Electrode_104</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0</v>
+      </c>
+      <c r="C105" t="n">
+        <v>0</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0</v>
+      </c>
+      <c r="G105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Electrode_105</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>0</v>
+      </c>
+      <c r="C106" t="n">
+        <v>0</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0</v>
+      </c>
+      <c r="G106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Electrode_106</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>0</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Electrode_107</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>0</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Electrode_108</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>0</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Electrode_109</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>0</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Electrode_110</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>0</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0</v>
+      </c>
+      <c r="G111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Electrode_111</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>0</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0</v>
+      </c>
+      <c r="G112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Electrode_112</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>0</v>
+      </c>
+      <c r="C113" t="n">
+        <v>0</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0</v>
+      </c>
+      <c r="G113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Electrode_113</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>0</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Electrode_114</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>0</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Electrode_115</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>0</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Electrode_116</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>0</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0</v>
+      </c>
+      <c r="G117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Electrode_117</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>0</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0</v>
+      </c>
+      <c r="G118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Electrode_118</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>0</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0</v>
+      </c>
+      <c r="G119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Electrode_119</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>0</v>
+      </c>
+      <c r="C120" t="n">
+        <v>0</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0</v>
+      </c>
+      <c r="G120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Electrode_120</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>0</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
i electrode is active
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>updated</t>
+          <t>active</t>
         </is>
       </c>
     </row>
@@ -491,9 +491,7 @@
       <c r="F2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -516,9 +514,7 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -541,9 +537,7 @@
       <c r="F4" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -566,9 +560,7 @@
       <c r="F5" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -591,9 +583,7 @@
       <c r="F6" t="n">
         <v>0</v>
       </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -616,9 +606,7 @@
       <c r="F7" t="n">
         <v>0</v>
       </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -641,9 +629,7 @@
       <c r="F8" t="n">
         <v>0</v>
       </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -666,9 +652,7 @@
       <c r="F9" t="n">
         <v>0</v>
       </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -691,9 +675,7 @@
       <c r="F10" t="n">
         <v>0</v>
       </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -716,9 +698,7 @@
       <c r="F11" t="n">
         <v>0</v>
       </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -729,7 +709,9 @@
       <c r="B12" t="n">
         <v>287</v>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
       <c r="D12" t="n">
         <v>-3.301043592334494e-05</v>
       </c>
@@ -752,7 +734,9 @@
       <c r="B13" t="n">
         <v>355</v>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
       <c r="D13" t="n">
         <v>-6.969021709859154e-05</v>
       </c>
@@ -775,7 +759,9 @@
       <c r="B14" t="n">
         <v>99</v>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
       <c r="D14" t="n">
         <v>2.583738818181818e-05</v>
       </c>
@@ -798,7 +784,9 @@
       <c r="B15" t="n">
         <v>651</v>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
       <c r="D15" t="n">
         <v>3.238886926267281e-05</v>
       </c>
@@ -871,7 +859,9 @@
       <c r="B18" t="n">
         <v>3</v>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
       <c r="D18" t="n">
         <v>-2.594931e-05</v>
       </c>
@@ -882,7 +872,7 @@
         <v>4</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -906,9 +896,7 @@
       <c r="F19" t="n">
         <v>0</v>
       </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
+      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -931,9 +919,7 @@
       <c r="F20" t="n">
         <v>0</v>
       </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
+      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -956,9 +942,7 @@
       <c r="F21" t="n">
         <v>0</v>
       </c>
-      <c r="G21" t="b">
-        <v>0</v>
-      </c>
+      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -981,9 +965,7 @@
       <c r="F22" t="n">
         <v>0</v>
       </c>
-      <c r="G22" t="b">
-        <v>0</v>
-      </c>
+      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1006,9 +988,7 @@
       <c r="F23" t="n">
         <v>0</v>
       </c>
-      <c r="G23" t="b">
-        <v>0</v>
-      </c>
+      <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1031,9 +1011,7 @@
       <c r="F24" t="n">
         <v>0</v>
       </c>
-      <c r="G24" t="b">
-        <v>0</v>
-      </c>
+      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1056,9 +1034,7 @@
       <c r="F25" t="n">
         <v>0</v>
       </c>
-      <c r="G25" t="b">
-        <v>0</v>
-      </c>
+      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1081,9 +1057,7 @@
       <c r="F26" t="n">
         <v>0</v>
       </c>
-      <c r="G26" t="b">
-        <v>0</v>
-      </c>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1106,9 +1080,7 @@
       <c r="F27" t="n">
         <v>0</v>
       </c>
-      <c r="G27" t="b">
-        <v>0</v>
-      </c>
+      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1131,9 +1103,7 @@
       <c r="F28" t="n">
         <v>0</v>
       </c>
-      <c r="G28" t="b">
-        <v>0</v>
-      </c>
+      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1156,9 +1126,7 @@
       <c r="F29" t="n">
         <v>0</v>
       </c>
-      <c r="G29" t="b">
-        <v>0</v>
-      </c>
+      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1181,9 +1149,7 @@
       <c r="F30" t="n">
         <v>0</v>
       </c>
-      <c r="G30" t="b">
-        <v>0</v>
-      </c>
+      <c r="G30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1206,9 +1172,7 @@
       <c r="F31" t="n">
         <v>0</v>
       </c>
-      <c r="G31" t="b">
-        <v>0</v>
-      </c>
+      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1231,9 +1195,7 @@
       <c r="F32" t="n">
         <v>0</v>
       </c>
-      <c r="G32" t="b">
-        <v>0</v>
-      </c>
+      <c r="G32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1256,9 +1218,7 @@
       <c r="F33" t="n">
         <v>0</v>
       </c>
-      <c r="G33" t="b">
-        <v>0</v>
-      </c>
+      <c r="G33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1281,9 +1241,7 @@
       <c r="F34" t="n">
         <v>0</v>
       </c>
-      <c r="G34" t="b">
-        <v>0</v>
-      </c>
+      <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1306,9 +1264,7 @@
       <c r="F35" t="n">
         <v>0</v>
       </c>
-      <c r="G35" t="b">
-        <v>0</v>
-      </c>
+      <c r="G35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1331,9 +1287,7 @@
       <c r="F36" t="n">
         <v>0</v>
       </c>
-      <c r="G36" t="b">
-        <v>0</v>
-      </c>
+      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1356,9 +1310,7 @@
       <c r="F37" t="n">
         <v>0</v>
       </c>
-      <c r="G37" t="b">
-        <v>0</v>
-      </c>
+      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1381,9 +1333,7 @@
       <c r="F38" t="n">
         <v>0</v>
       </c>
-      <c r="G38" t="b">
-        <v>0</v>
-      </c>
+      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1406,9 +1356,7 @@
       <c r="F39" t="n">
         <v>0</v>
       </c>
-      <c r="G39" t="b">
-        <v>0</v>
-      </c>
+      <c r="G39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1431,9 +1379,7 @@
       <c r="F40" t="n">
         <v>0</v>
       </c>
-      <c r="G40" t="b">
-        <v>0</v>
-      </c>
+      <c r="G40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1456,9 +1402,7 @@
       <c r="F41" t="n">
         <v>0</v>
       </c>
-      <c r="G41" t="b">
-        <v>0</v>
-      </c>
+      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1481,9 +1425,7 @@
       <c r="F42" t="n">
         <v>0</v>
       </c>
-      <c r="G42" t="b">
-        <v>0</v>
-      </c>
+      <c r="G42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1506,9 +1448,7 @@
       <c r="F43" t="n">
         <v>0</v>
       </c>
-      <c r="G43" t="b">
-        <v>0</v>
-      </c>
+      <c r="G43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1531,9 +1471,7 @@
       <c r="F44" t="n">
         <v>0</v>
       </c>
-      <c r="G44" t="b">
-        <v>0</v>
-      </c>
+      <c r="G44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1556,9 +1494,7 @@
       <c r="F45" t="n">
         <v>0</v>
       </c>
-      <c r="G45" t="b">
-        <v>0</v>
-      </c>
+      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1581,9 +1517,7 @@
       <c r="F46" t="n">
         <v>0</v>
       </c>
-      <c r="G46" t="b">
-        <v>0</v>
-      </c>
+      <c r="G46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1606,9 +1540,7 @@
       <c r="F47" t="n">
         <v>0</v>
       </c>
-      <c r="G47" t="b">
-        <v>0</v>
-      </c>
+      <c r="G47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1631,9 +1563,7 @@
       <c r="F48" t="n">
         <v>0</v>
       </c>
-      <c r="G48" t="b">
-        <v>0</v>
-      </c>
+      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1656,9 +1586,7 @@
       <c r="F49" t="n">
         <v>0</v>
       </c>
-      <c r="G49" t="b">
-        <v>0</v>
-      </c>
+      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1681,9 +1609,7 @@
       <c r="F50" t="n">
         <v>0</v>
       </c>
-      <c r="G50" t="b">
-        <v>0</v>
-      </c>
+      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1706,9 +1632,7 @@
       <c r="F51" t="n">
         <v>0</v>
       </c>
-      <c r="G51" t="b">
-        <v>0</v>
-      </c>
+      <c r="G51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1731,9 +1655,7 @@
       <c r="F52" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="b">
-        <v>0</v>
-      </c>
+      <c r="G52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1756,9 +1678,7 @@
       <c r="F53" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="b">
-        <v>0</v>
-      </c>
+      <c r="G53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1781,9 +1701,7 @@
       <c r="F54" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="b">
-        <v>0</v>
-      </c>
+      <c r="G54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1806,9 +1724,7 @@
       <c r="F55" t="n">
         <v>0</v>
       </c>
-      <c r="G55" t="b">
-        <v>0</v>
-      </c>
+      <c r="G55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1831,9 +1747,7 @@
       <c r="F56" t="n">
         <v>0</v>
       </c>
-      <c r="G56" t="b">
-        <v>0</v>
-      </c>
+      <c r="G56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1856,9 +1770,7 @@
       <c r="F57" t="n">
         <v>0</v>
       </c>
-      <c r="G57" t="b">
-        <v>0</v>
-      </c>
+      <c r="G57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1881,9 +1793,7 @@
       <c r="F58" t="n">
         <v>0</v>
       </c>
-      <c r="G58" t="b">
-        <v>0</v>
-      </c>
+      <c r="G58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1906,9 +1816,7 @@
       <c r="F59" t="n">
         <v>0</v>
       </c>
-      <c r="G59" t="b">
-        <v>0</v>
-      </c>
+      <c r="G59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1931,9 +1839,7 @@
       <c r="F60" t="n">
         <v>0</v>
       </c>
-      <c r="G60" t="b">
-        <v>0</v>
-      </c>
+      <c r="G60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1956,9 +1862,7 @@
       <c r="F61" t="n">
         <v>0</v>
       </c>
-      <c r="G61" t="b">
-        <v>0</v>
-      </c>
+      <c r="G61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1981,9 +1885,7 @@
       <c r="F62" t="n">
         <v>0</v>
       </c>
-      <c r="G62" t="b">
-        <v>0</v>
-      </c>
+      <c r="G62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2006,9 +1908,7 @@
       <c r="F63" t="n">
         <v>0</v>
       </c>
-      <c r="G63" t="b">
-        <v>0</v>
-      </c>
+      <c r="G63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2031,9 +1931,7 @@
       <c r="F64" t="n">
         <v>0</v>
       </c>
-      <c r="G64" t="b">
-        <v>0</v>
-      </c>
+      <c r="G64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2056,9 +1954,7 @@
       <c r="F65" t="n">
         <v>0</v>
       </c>
-      <c r="G65" t="b">
-        <v>0</v>
-      </c>
+      <c r="G65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2081,9 +1977,7 @@
       <c r="F66" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="b">
-        <v>0</v>
-      </c>
+      <c r="G66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2106,9 +2000,7 @@
       <c r="F67" t="n">
         <v>0</v>
       </c>
-      <c r="G67" t="b">
-        <v>0</v>
-      </c>
+      <c r="G67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2131,9 +2023,7 @@
       <c r="F68" t="n">
         <v>0</v>
       </c>
-      <c r="G68" t="b">
-        <v>0</v>
-      </c>
+      <c r="G68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2156,9 +2046,7 @@
       <c r="F69" t="n">
         <v>0</v>
       </c>
-      <c r="G69" t="b">
-        <v>0</v>
-      </c>
+      <c r="G69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2181,9 +2069,7 @@
       <c r="F70" t="n">
         <v>0</v>
       </c>
-      <c r="G70" t="b">
-        <v>0</v>
-      </c>
+      <c r="G70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2206,9 +2092,7 @@
       <c r="F71" t="n">
         <v>0</v>
       </c>
-      <c r="G71" t="b">
-        <v>0</v>
-      </c>
+      <c r="G71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2231,9 +2115,7 @@
       <c r="F72" t="n">
         <v>0</v>
       </c>
-      <c r="G72" t="b">
-        <v>0</v>
-      </c>
+      <c r="G72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2256,9 +2138,7 @@
       <c r="F73" t="n">
         <v>0</v>
       </c>
-      <c r="G73" t="b">
-        <v>0</v>
-      </c>
+      <c r="G73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2281,9 +2161,7 @@
       <c r="F74" t="n">
         <v>0</v>
       </c>
-      <c r="G74" t="b">
-        <v>0</v>
-      </c>
+      <c r="G74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2306,9 +2184,7 @@
       <c r="F75" t="n">
         <v>0</v>
       </c>
-      <c r="G75" t="b">
-        <v>0</v>
-      </c>
+      <c r="G75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2331,9 +2207,7 @@
       <c r="F76" t="n">
         <v>0</v>
       </c>
-      <c r="G76" t="b">
-        <v>0</v>
-      </c>
+      <c r="G76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2356,9 +2230,7 @@
       <c r="F77" t="n">
         <v>0</v>
       </c>
-      <c r="G77" t="b">
-        <v>0</v>
-      </c>
+      <c r="G77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2381,9 +2253,7 @@
       <c r="F78" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="b">
-        <v>0</v>
-      </c>
+      <c r="G78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2406,9 +2276,7 @@
       <c r="F79" t="n">
         <v>0</v>
       </c>
-      <c r="G79" t="b">
-        <v>0</v>
-      </c>
+      <c r="G79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2431,9 +2299,7 @@
       <c r="F80" t="n">
         <v>0</v>
       </c>
-      <c r="G80" t="b">
-        <v>0</v>
-      </c>
+      <c r="G80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2456,9 +2322,7 @@
       <c r="F81" t="n">
         <v>0</v>
       </c>
-      <c r="G81" t="b">
-        <v>0</v>
-      </c>
+      <c r="G81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2481,9 +2345,7 @@
       <c r="F82" t="n">
         <v>0</v>
       </c>
-      <c r="G82" t="b">
-        <v>0</v>
-      </c>
+      <c r="G82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2506,9 +2368,7 @@
       <c r="F83" t="n">
         <v>0</v>
       </c>
-      <c r="G83" t="b">
-        <v>0</v>
-      </c>
+      <c r="G83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2531,9 +2391,7 @@
       <c r="F84" t="n">
         <v>0</v>
       </c>
-      <c r="G84" t="b">
-        <v>0</v>
-      </c>
+      <c r="G84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2556,9 +2414,7 @@
       <c r="F85" t="n">
         <v>0</v>
       </c>
-      <c r="G85" t="b">
-        <v>0</v>
-      </c>
+      <c r="G85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2581,9 +2437,7 @@
       <c r="F86" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="b">
-        <v>0</v>
-      </c>
+      <c r="G86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2606,9 +2460,7 @@
       <c r="F87" t="n">
         <v>0</v>
       </c>
-      <c r="G87" t="b">
-        <v>0</v>
-      </c>
+      <c r="G87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2631,9 +2483,7 @@
       <c r="F88" t="n">
         <v>0</v>
       </c>
-      <c r="G88" t="b">
-        <v>0</v>
-      </c>
+      <c r="G88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2656,9 +2506,7 @@
       <c r="F89" t="n">
         <v>0</v>
       </c>
-      <c r="G89" t="b">
-        <v>0</v>
-      </c>
+      <c r="G89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2681,9 +2529,7 @@
       <c r="F90" t="n">
         <v>0</v>
       </c>
-      <c r="G90" t="b">
-        <v>0</v>
-      </c>
+      <c r="G90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2706,9 +2552,7 @@
       <c r="F91" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="b">
-        <v>0</v>
-      </c>
+      <c r="G91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2731,9 +2575,7 @@
       <c r="F92" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="b">
-        <v>0</v>
-      </c>
+      <c r="G92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2756,9 +2598,7 @@
       <c r="F93" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="b">
-        <v>0</v>
-      </c>
+      <c r="G93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2781,9 +2621,7 @@
       <c r="F94" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="b">
-        <v>0</v>
-      </c>
+      <c r="G94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2806,9 +2644,7 @@
       <c r="F95" t="n">
         <v>0</v>
       </c>
-      <c r="G95" t="b">
-        <v>0</v>
-      </c>
+      <c r="G95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2831,9 +2667,7 @@
       <c r="F96" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="b">
-        <v>0</v>
-      </c>
+      <c r="G96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2856,9 +2690,7 @@
       <c r="F97" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="b">
-        <v>0</v>
-      </c>
+      <c r="G97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2881,9 +2713,7 @@
       <c r="F98" t="n">
         <v>0</v>
       </c>
-      <c r="G98" t="b">
-        <v>0</v>
-      </c>
+      <c r="G98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2906,9 +2736,7 @@
       <c r="F99" t="n">
         <v>0</v>
       </c>
-      <c r="G99" t="b">
-        <v>0</v>
-      </c>
+      <c r="G99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2931,9 +2759,7 @@
       <c r="F100" t="n">
         <v>0</v>
       </c>
-      <c r="G100" t="b">
-        <v>0</v>
-      </c>
+      <c r="G100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2956,9 +2782,7 @@
       <c r="F101" t="n">
         <v>0</v>
       </c>
-      <c r="G101" t="b">
-        <v>0</v>
-      </c>
+      <c r="G101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2981,9 +2805,7 @@
       <c r="F102" t="n">
         <v>0</v>
       </c>
-      <c r="G102" t="b">
-        <v>0</v>
-      </c>
+      <c r="G102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3006,9 +2828,7 @@
       <c r="F103" t="n">
         <v>0</v>
       </c>
-      <c r="G103" t="b">
-        <v>0</v>
-      </c>
+      <c r="G103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3031,9 +2851,7 @@
       <c r="F104" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="b">
-        <v>0</v>
-      </c>
+      <c r="G104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3056,9 +2874,7 @@
       <c r="F105" t="n">
         <v>0</v>
       </c>
-      <c r="G105" t="b">
-        <v>0</v>
-      </c>
+      <c r="G105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3081,9 +2897,7 @@
       <c r="F106" t="n">
         <v>0</v>
       </c>
-      <c r="G106" t="b">
-        <v>0</v>
-      </c>
+      <c r="G106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3106,9 +2920,7 @@
       <c r="F107" t="n">
         <v>0</v>
       </c>
-      <c r="G107" t="b">
-        <v>0</v>
-      </c>
+      <c r="G107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3131,9 +2943,7 @@
       <c r="F108" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="b">
-        <v>0</v>
-      </c>
+      <c r="G108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3156,9 +2966,7 @@
       <c r="F109" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="b">
-        <v>0</v>
-      </c>
+      <c r="G109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3181,9 +2989,7 @@
       <c r="F110" t="n">
         <v>0</v>
       </c>
-      <c r="G110" t="b">
-        <v>0</v>
-      </c>
+      <c r="G110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3206,9 +3012,7 @@
       <c r="F111" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="b">
-        <v>0</v>
-      </c>
+      <c r="G111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3231,9 +3035,7 @@
       <c r="F112" t="n">
         <v>0</v>
       </c>
-      <c r="G112" t="b">
-        <v>0</v>
-      </c>
+      <c r="G112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3256,9 +3058,7 @@
       <c r="F113" t="n">
         <v>0</v>
       </c>
-      <c r="G113" t="b">
-        <v>0</v>
-      </c>
+      <c r="G113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3281,9 +3081,7 @@
       <c r="F114" t="n">
         <v>0</v>
       </c>
-      <c r="G114" t="b">
-        <v>0</v>
-      </c>
+      <c r="G114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3306,9 +3104,7 @@
       <c r="F115" t="n">
         <v>0</v>
       </c>
-      <c r="G115" t="b">
-        <v>0</v>
-      </c>
+      <c r="G115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3331,9 +3127,7 @@
       <c r="F116" t="n">
         <v>0</v>
       </c>
-      <c r="G116" t="b">
-        <v>0</v>
-      </c>
+      <c r="G116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3356,9 +3150,7 @@
       <c r="F117" t="n">
         <v>0</v>
       </c>
-      <c r="G117" t="b">
-        <v>0</v>
-      </c>
+      <c r="G117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3381,9 +3173,7 @@
       <c r="F118" t="n">
         <v>0</v>
       </c>
-      <c r="G118" t="b">
-        <v>0</v>
-      </c>
+      <c r="G118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3406,9 +3196,7 @@
       <c r="F119" t="n">
         <v>0</v>
       </c>
-      <c r="G119" t="b">
-        <v>0</v>
-      </c>
+      <c r="G119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3431,9 +3219,7 @@
       <c r="F120" t="n">
         <v>0</v>
       </c>
-      <c r="G120" t="b">
-        <v>0</v>
-      </c>
+      <c r="G120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3456,9 +3242,7 @@
       <c r="F121" t="n">
         <v>0</v>
       </c>
-      <c r="G121" t="b">
-        <v>0</v>
-      </c>
+      <c r="G121" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>